<commit_message>
EMail API added after testing
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -61,31 +61,13 @@
     <t>prof.amit.arora@gmail.com</t>
   </si>
   <si>
-    <t>cus_KPstgGGPqnOQjg</t>
-  </si>
-  <si>
-    <t>cus_KPst3cDQtQtNiK</t>
-  </si>
-  <si>
-    <t>cus_KPstiT62aEUEyi</t>
-  </si>
-  <si>
-    <t>cus_KPg82hmMUoLftD</t>
-  </si>
-  <si>
-    <t>cus_KPg8mcTOmJreyh</t>
-  </si>
-  <si>
-    <t>cus_KPg8vduROpIphp</t>
-  </si>
-  <si>
-    <t>cus_KPfZoZTDvxLCwB</t>
-  </si>
-  <si>
-    <t>cus_KPfZzI1I5MrEfJ</t>
-  </si>
-  <si>
-    <t>cus_KPfZG0RNY9NZKV</t>
+    <t>cus_KQ6aaMpTMkZP9V</t>
+  </si>
+  <si>
+    <t>cus_KQ6ayxL6jsGJ8c</t>
+  </si>
+  <si>
+    <t>cus_KQ6aP84xmpHq5P</t>
   </si>
 </sst>
 </file>
@@ -430,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A13" sqref="A13:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -544,36 +526,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>

</xml_diff>